<commit_message>
adjust frequency plan switches to embrace AU915
</commit_message>
<xml_diff>
--- a/Docs/rfsel.xlsx
+++ b/Docs/rfsel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rozzie/dev/blues/sparrow/Docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ray\dev\sparrow-lora\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81B8BFC3-106D-9E4F-A531-7E1F042BF0E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17EE15E2-D5B4-4A9C-B181-3DF7DE4AE2B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2740" yWindow="3100" windowWidth="23620" windowHeight="20320" xr2:uid="{C7CECD9E-F68B-984D-984F-46888768E6A5}"/>
+    <workbookView xWindow="3735" yWindow="5280" windowWidth="28800" windowHeight="17235" xr2:uid="{C7CECD9E-F68B-984D-984F-46888768E6A5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -72,9 +72,6 @@
     <t>GPIO1</t>
   </si>
   <si>
-    <t>US915 &amp; AU915</t>
-  </si>
-  <si>
     <t>AS923</t>
   </si>
   <si>
@@ -90,9 +87,6 @@
     <t>RU864</t>
   </si>
   <si>
-    <t>CN779</t>
-  </si>
-  <si>
     <t>CN470</t>
   </si>
   <si>
@@ -118,6 +112,12 @@
   </si>
   <si>
     <t>Kohms</t>
+  </si>
+  <si>
+    <t>US915</t>
+  </si>
+  <si>
+    <t>AU915</t>
   </si>
 </sst>
 </file>
@@ -127,7 +127,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -188,21 +188,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -521,18 +521,18 @@
   <dimension ref="B2:R29"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="O25" sqref="O25"/>
+      <selection activeCell="O28" sqref="O28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="2" max="10" width="8.83203125" customWidth="1"/>
+    <col min="2" max="10" width="8.875" customWidth="1"/>
     <col min="11" max="11" width="9.5" customWidth="1"/>
-    <col min="12" max="12" width="15.6640625" customWidth="1"/>
-    <col min="14" max="14" width="4.83203125" customWidth="1"/>
+    <col min="12" max="12" width="15.625" customWidth="1"/>
+    <col min="14" max="14" width="4.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:18" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:18" s="3" customFormat="1">
       <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
@@ -555,7 +555,7 @@
         <v>10</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
@@ -565,7 +565,7 @@
       <c r="Q2" s="4"/>
       <c r="R2" s="4"/>
     </row>
-    <row r="3" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:18">
       <c r="B3" s="1" t="s">
         <v>9</v>
       </c>
@@ -588,7 +588,7 @@
         <v>0</v>
       </c>
       <c r="I3" s="6">
-        <f>IF(AND(B3="ON",C3="ON"),$J$17,0)+IF(AND(D3="ON",E3="ON"),$J$17,0)</f>
+        <f t="shared" ref="I3:I18" si="0">IF(AND(B3="ON",C3="ON"),$J$17,0)+IF(AND(D3="ON",E3="ON"),$J$17,0)</f>
         <v>0</v>
       </c>
       <c r="J3" s="1"/>
@@ -599,7 +599,7 @@
       <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
     </row>
-    <row r="4" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:18">
       <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
@@ -622,7 +622,7 @@
         <v>1</v>
       </c>
       <c r="I4" s="6">
-        <f>IF(AND(B4="ON",C4="ON"),$J$17,0)+IF(AND(D4="ON",E4="ON"),$J$17,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J4" s="1"/>
@@ -633,7 +633,7 @@
       <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
     </row>
-    <row r="5" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:18">
       <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
@@ -656,7 +656,7 @@
         <v>2</v>
       </c>
       <c r="I5" s="6">
-        <f>IF(AND(B5="ON",C5="ON"),$J$17,0)+IF(AND(D5="ON",E5="ON"),$J$17,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J5" s="1"/>
@@ -666,7 +666,7 @@
       <c r="Q5" s="1"/>
       <c r="R5" s="1"/>
     </row>
-    <row r="6" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:18">
       <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
@@ -689,7 +689,7 @@
         <v>1</v>
       </c>
       <c r="I6" s="6">
-        <f>IF(AND(B6="ON",C6="ON"),$J$17,0)+IF(AND(D6="ON",E6="ON"),$J$17,0)</f>
+        <f t="shared" si="0"/>
         <v>3.2673267326732671</v>
       </c>
       <c r="J6" s="1"/>
@@ -701,7 +701,7 @@
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
     </row>
-    <row r="7" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:18">
       <c r="B7" s="1" t="s">
         <v>9</v>
       </c>
@@ -724,7 +724,7 @@
         <v>3</v>
       </c>
       <c r="I7" s="6">
-        <f>IF(AND(B7="ON",C7="ON"),$J$17,0)+IF(AND(D7="ON",E7="ON"),$J$17,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K7" s="2"/>
@@ -735,7 +735,7 @@
       <c r="Q7" s="1"/>
       <c r="R7" s="1"/>
     </row>
-    <row r="8" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:18">
       <c r="B8" s="1" t="s">
         <v>6</v>
       </c>
@@ -758,7 +758,7 @@
         <v>4</v>
       </c>
       <c r="I8" s="6">
-        <f>IF(AND(B8="ON",C8="ON"),$J$17,0)+IF(AND(D8="ON",E8="ON"),$J$17,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J8" s="1"/>
@@ -770,7 +770,7 @@
       <c r="Q8" s="1"/>
       <c r="R8" s="1"/>
     </row>
-    <row r="9" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:18">
       <c r="B9" s="1" t="s">
         <v>9</v>
       </c>
@@ -793,7 +793,7 @@
         <v>5</v>
       </c>
       <c r="I9" s="6">
-        <f>IF(AND(B9="ON",C9="ON"),$J$17,0)+IF(AND(D9="ON",E9="ON"),$J$17,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J9" s="1"/>
@@ -805,7 +805,7 @@
       <c r="Q9" s="1"/>
       <c r="R9" s="1"/>
     </row>
-    <row r="10" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:18">
       <c r="B10" s="1" t="s">
         <v>6</v>
       </c>
@@ -828,7 +828,7 @@
         <v>4</v>
       </c>
       <c r="I10" s="6">
-        <f>IF(AND(B10="ON",C10="ON"),$J$17,0)+IF(AND(D10="ON",E10="ON"),$J$17,0)</f>
+        <f t="shared" si="0"/>
         <v>3.2673267326732671</v>
       </c>
       <c r="J10" s="1"/>
@@ -840,7 +840,7 @@
       <c r="Q10" s="1"/>
       <c r="R10" s="1"/>
     </row>
-    <row r="11" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:18">
       <c r="B11" s="1" t="s">
         <v>9</v>
       </c>
@@ -863,7 +863,7 @@
         <v>6</v>
       </c>
       <c r="I11" s="6">
-        <f>IF(AND(B11="ON",C11="ON"),$J$17,0)+IF(AND(D11="ON",E11="ON"),$J$17,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J11" s="1"/>
@@ -875,7 +875,7 @@
       <c r="Q11" s="1"/>
       <c r="R11" s="1"/>
     </row>
-    <row r="12" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:18">
       <c r="B12" s="1" t="s">
         <v>6</v>
       </c>
@@ -898,11 +898,11 @@
         <v>7</v>
       </c>
       <c r="I12" s="6">
-        <f>IF(AND(B12="ON",C12="ON"),$J$17,0)+IF(AND(D12="ON",E12="ON"),$J$17,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="2:18" x14ac:dyDescent="0.2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:18">
       <c r="B13" s="1" t="s">
         <v>9</v>
       </c>
@@ -925,11 +925,11 @@
         <v>8</v>
       </c>
       <c r="I13" s="6">
-        <f>IF(AND(B13="ON",C13="ON"),$J$17,0)+IF(AND(D13="ON",E13="ON"),$J$17,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="2:18" x14ac:dyDescent="0.2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:18">
       <c r="B14" s="1" t="s">
         <v>6</v>
       </c>
@@ -952,17 +952,17 @@
         <v>7</v>
       </c>
       <c r="I14" s="6">
-        <f>IF(AND(B14="ON",C14="ON"),$J$17,0)+IF(AND(D14="ON",E14="ON"),$J$17,0)</f>
+        <f t="shared" si="0"/>
         <v>3.2673267326732671</v>
       </c>
       <c r="J14">
         <v>3.3</v>
       </c>
-      <c r="K14" s="11" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="15" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="K14" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="2:18">
       <c r="B15" s="1" t="s">
         <v>9</v>
       </c>
@@ -985,17 +985,17 @@
         <v>3</v>
       </c>
       <c r="I15" s="6">
-        <f>IF(AND(B15="ON",C15="ON"),$J$17,0)+IF(AND(D15="ON",E15="ON"),$J$17,0)</f>
+        <f t="shared" si="0"/>
         <v>3.2673267326732671</v>
       </c>
-      <c r="J15" s="10">
+      <c r="J15" s="7">
         <v>10</v>
       </c>
-      <c r="K15" s="11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="16" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="K15" s="8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="2:18">
       <c r="B16" s="1" t="s">
         <v>6</v>
       </c>
@@ -1018,17 +1018,17 @@
         <v>4</v>
       </c>
       <c r="I16" s="6">
-        <f>IF(AND(B16="ON",C16="ON"),$J$17,0)+IF(AND(D16="ON",E16="ON"),$J$17,0)</f>
+        <f t="shared" si="0"/>
         <v>3.2673267326732671</v>
       </c>
-      <c r="J16" s="10">
+      <c r="J16" s="7">
         <v>1000</v>
       </c>
-      <c r="K16" s="11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="K16" s="8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12">
       <c r="B17" s="1" t="s">
         <v>9</v>
       </c>
@@ -1051,18 +1051,18 @@
         <v>5</v>
       </c>
       <c r="I17" s="6">
-        <f>IF(AND(B17="ON",C17="ON"),$J$17,0)+IF(AND(D17="ON",E17="ON"),$J$17,0)</f>
+        <f t="shared" si="0"/>
         <v>3.2673267326732671</v>
       </c>
-      <c r="J17" s="12">
+      <c r="J17" s="9">
         <f>(J14/(1000*J15+1000*J16))*1000000</f>
         <v>3.2673267326732671</v>
       </c>
       <c r="K17" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12">
       <c r="B18" s="1" t="s">
         <v>6</v>
       </c>
@@ -1085,22 +1085,22 @@
         <v>4</v>
       </c>
       <c r="I18" s="6">
-        <f>IF(AND(B18="ON",C18="ON"),$J$17,0)+IF(AND(D18="ON",E18="ON"),$J$17,0)</f>
+        <f t="shared" si="0"/>
         <v>6.5346534653465342</v>
       </c>
     </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:12">
       <c r="B20" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C20" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="F20" s="7"/>
+      <c r="F20" s="11"/>
       <c r="G20" s="4" t="s">
         <v>0</v>
       </c>
@@ -1114,22 +1114,22 @@
         <v>3</v>
       </c>
       <c r="K20" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="L20" s="5"/>
     </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:12">
       <c r="B21" s="1">
         <v>0</v>
       </c>
-      <c r="C21" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8">
+      <c r="C21" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10">
         <v>915000000</v>
       </c>
-      <c r="F21" s="8"/>
+      <c r="F21" s="10"/>
       <c r="G21" s="1" t="s">
         <v>9</v>
       </c>
@@ -1143,22 +1143,22 @@
         <v>9</v>
       </c>
       <c r="K21" s="6">
-        <f>IF(AND(G21="ON",H21="ON"),$J$17,0)+IF(AND(I21="ON",J21="ON"),$J$17,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.2">
+        <f t="shared" ref="K21:K29" si="1">IF(AND(G21="ON",H21="ON"),$J$17,0)+IF(AND(I21="ON",J21="ON"),$J$17,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="2:12">
       <c r="B22" s="1">
         <v>1</v>
       </c>
-      <c r="C22" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="D22" s="9"/>
-      <c r="E22" s="8">
+      <c r="C22" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D22" s="12"/>
+      <c r="E22" s="10">
         <v>923000000</v>
       </c>
-      <c r="F22" s="8"/>
+      <c r="F22" s="10"/>
       <c r="G22" s="1" t="s">
         <v>6</v>
       </c>
@@ -1172,22 +1172,22 @@
         <v>9</v>
       </c>
       <c r="K22" s="6">
-        <f>IF(AND(G22="ON",H22="ON"),$J$17,0)+IF(AND(I22="ON",J22="ON"),$J$17,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="2:12">
       <c r="B23" s="1">
         <v>2</v>
       </c>
-      <c r="C23" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D23" s="8"/>
-      <c r="E23" s="8">
+      <c r="C23" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10">
         <v>920000000</v>
       </c>
-      <c r="F23" s="8"/>
+      <c r="F23" s="10"/>
       <c r="G23" s="1" t="s">
         <v>9</v>
       </c>
@@ -1201,22 +1201,22 @@
         <v>9</v>
       </c>
       <c r="K23" s="6">
-        <f>IF(AND(G23="ON",H23="ON"),$J$17,0)+IF(AND(I23="ON",J23="ON"),$J$17,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="2:12">
       <c r="B24" s="1">
         <v>3</v>
       </c>
-      <c r="C24" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D24" s="8"/>
-      <c r="E24" s="8">
+      <c r="C24" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D24" s="10"/>
+      <c r="E24" s="10">
         <v>865000000</v>
       </c>
-      <c r="F24" s="8"/>
+      <c r="F24" s="10"/>
       <c r="G24" s="1" t="s">
         <v>9</v>
       </c>
@@ -1230,22 +1230,22 @@
         <v>9</v>
       </c>
       <c r="K24" s="6">
-        <f>IF(AND(G24="ON",H24="ON"),$J$17,0)+IF(AND(I24="ON",J24="ON"),$J$17,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="2:12">
       <c r="B25" s="1">
         <v>4</v>
       </c>
-      <c r="C25" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D25" s="8"/>
-      <c r="E25" s="8">
+      <c r="C25" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10">
         <v>868000000</v>
       </c>
-      <c r="F25" s="8"/>
+      <c r="F25" s="10"/>
       <c r="G25" s="1" t="s">
         <v>6</v>
       </c>
@@ -1259,22 +1259,22 @@
         <v>9</v>
       </c>
       <c r="K25" s="6">
-        <f>IF(AND(G25="ON",H25="ON"),$J$17,0)+IF(AND(I25="ON",J25="ON"),$J$17,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="2:12">
       <c r="B26" s="1">
         <v>5</v>
       </c>
-      <c r="C26" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D26" s="8"/>
-      <c r="E26" s="8">
+      <c r="C26" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D26" s="10"/>
+      <c r="E26" s="10">
         <v>864000000</v>
       </c>
-      <c r="F26" s="8"/>
+      <c r="F26" s="10"/>
       <c r="G26" s="1" t="s">
         <v>9</v>
       </c>
@@ -1288,22 +1288,22 @@
         <v>9</v>
       </c>
       <c r="K26" s="6">
-        <f>IF(AND(G26="ON",H26="ON"),$J$17,0)+IF(AND(I26="ON",J26="ON"),$J$17,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="2:12">
       <c r="B27" s="1">
         <v>6</v>
       </c>
-      <c r="C27" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="D27" s="8"/>
-      <c r="E27" s="8">
+      <c r="C27" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D27" s="10"/>
+      <c r="E27" s="10">
         <v>779000000</v>
       </c>
-      <c r="F27" s="8"/>
+      <c r="F27" s="10"/>
       <c r="G27" s="1" t="s">
         <v>9</v>
       </c>
@@ -1317,22 +1317,22 @@
         <v>6</v>
       </c>
       <c r="K27" s="6">
-        <f>IF(AND(G27="ON",H27="ON"),$J$17,0)+IF(AND(I27="ON",J27="ON"),$J$17,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="2:12">
       <c r="B28" s="1">
         <v>7</v>
       </c>
-      <c r="C28" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="D28" s="8"/>
-      <c r="E28" s="8">
+      <c r="C28" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D28" s="10"/>
+      <c r="E28" s="10">
         <v>470000000</v>
       </c>
-      <c r="F28" s="8"/>
+      <c r="F28" s="10"/>
       <c r="G28" s="1" t="s">
         <v>6</v>
       </c>
@@ -1346,22 +1346,22 @@
         <v>6</v>
       </c>
       <c r="K28" s="6">
-        <f>IF(AND(G28="ON",H28="ON"),$J$17,0)+IF(AND(I28="ON",J28="ON"),$J$17,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="2:12">
       <c r="B29" s="1">
         <v>8</v>
       </c>
-      <c r="C29" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D29" s="8"/>
-      <c r="E29" s="8">
+      <c r="C29" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D29" s="10"/>
+      <c r="E29" s="10">
         <v>433000000</v>
       </c>
-      <c r="F29" s="8"/>
+      <c r="F29" s="10"/>
       <c r="G29" s="1" t="s">
         <v>9</v>
       </c>
@@ -1375,12 +1375,16 @@
         <v>6</v>
       </c>
       <c r="K29" s="6">
-        <f>IF(AND(G29="ON",H29="ON"),$J$17,0)+IF(AND(I29="ON",J29="ON"),$J$17,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="C28:D28"/>
     <mergeCell ref="C29:D29"/>
     <mergeCell ref="E28:F28"/>
     <mergeCell ref="E29:F29"/>
@@ -1397,10 +1401,6 @@
     <mergeCell ref="E25:F25"/>
     <mergeCell ref="E24:F24"/>
     <mergeCell ref="E20:F20"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="C28:D28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>